<commit_message>
Revert "Standardized data organization"
This reverts commit 650ba6aab4adad159d86faa841dc4a4c9a276fe5.
</commit_message>
<xml_diff>
--- a/experiments/20161104-pol-assay-high-throughput/20161115-highthroughput-test-1st-scan.xlsx
+++ b/experiments/20161104-pol-assay-high-throughput/20161115-highthroughput-test-1st-scan.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,14 +24,245 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="106">
   <si>
     <t>Well</t>
   </si>
   <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A01</t>
+  </si>
+  <si>
+    <t>Assay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A12</t>
+  </si>
+  <si>
     <t>Luminescence</t>
   </si>
   <si>
+    <t>Well Type (Transfection)</t>
+  </si>
+  <si>
+    <t>Date (Scan)</t>
+  </si>
+  <si>
     <t>Mock</t>
   </si>
   <si>
@@ -93,6 +323,12 @@
     <t>L16</t>
   </si>
   <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>pcD</t>
+  </si>
+  <si>
     <t>1:2</t>
   </si>
   <si>
@@ -106,21 +342,6 @@
   </si>
   <si>
     <t>1:32</t>
-  </si>
-  <si>
-    <t>SampleID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Well Type</t>
-  </si>
-  <si>
-    <t>Replicate</t>
-  </si>
-  <si>
-    <t>PCD</t>
   </si>
 </sst>
 </file>
@@ -439,53 +660,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
     <col min="6" max="6" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1</v>
+        <v>20161115</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>20161115</v>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
       </c>
       <c r="F2">
         <v>-479.07499999999999</v>
@@ -493,19 +714,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>20161115</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
         <v>12</v>
       </c>
-      <c r="E3">
-        <v>20161115</v>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
       </c>
       <c r="F3">
         <v>572.37800000000004</v>
@@ -513,19 +734,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>20161115</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>20161115</v>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
       </c>
       <c r="F4">
         <v>1234820</v>
@@ -533,19 +754,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
+        <v>20161115</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
         <v>12</v>
       </c>
-      <c r="E5">
-        <v>20161115</v>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
       </c>
       <c r="F5">
         <v>1022020</v>
@@ -553,19 +774,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>20161115</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
         <v>12</v>
       </c>
-      <c r="E6">
-        <v>20161115</v>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
       </c>
       <c r="F6">
         <v>253.322</v>
@@ -573,19 +794,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>20161115</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
         <v>12</v>
       </c>
-      <c r="E7">
-        <v>20161115</v>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
       </c>
       <c r="F7">
         <v>168.86</v>
@@ -593,19 +814,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>20161115</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
         <v>12</v>
       </c>
-      <c r="E8">
-        <v>20161115</v>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
       </c>
       <c r="F8">
         <v>220.59899999999999</v>
@@ -613,19 +834,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>20161115</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
         <v>12</v>
       </c>
-      <c r="E9">
-        <v>20161115</v>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>86</v>
       </c>
       <c r="F9">
         <v>135.18199999999999</v>
@@ -633,19 +854,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>20161115</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
         <v>12</v>
       </c>
-      <c r="E10">
-        <v>20161115</v>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
       </c>
       <c r="F10">
         <v>485.8</v>
@@ -653,19 +874,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>20161115</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
         <v>12</v>
       </c>
-      <c r="E11">
-        <v>20161115</v>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
       </c>
       <c r="F11">
         <v>52.189300000000003</v>
@@ -673,19 +894,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>20161115</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12">
         <v>12</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <v>20161115</v>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
       </c>
       <c r="F12">
         <v>165.06</v>
@@ -693,19 +914,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
+        <v>20161115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>20161115</v>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
       </c>
       <c r="F13">
         <v>-200.79</v>
@@ -713,19 +934,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>13</v>
+        <v>20161115</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>96</v>
-      </c>
-      <c r="E14">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
       </c>
       <c r="F14">
         <v>809.08199999999999</v>
@@ -733,19 +954,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
+        <v>20161115</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>96</v>
-      </c>
-      <c r="E15">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>92</v>
       </c>
       <c r="F15">
         <v>-14.370699999999999</v>
@@ -753,19 +974,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>15</v>
+        <v>20161115</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>96</v>
-      </c>
-      <c r="E16">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>93</v>
       </c>
       <c r="F16">
         <v>-464.00799999999998</v>
@@ -773,19 +994,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>16</v>
+        <v>20161115</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>96</v>
-      </c>
-      <c r="E17">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
       </c>
       <c r="F17">
         <v>-40.953899999999997</v>
@@ -793,19 +1014,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>17</v>
+        <v>20161115</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>96</v>
-      </c>
-      <c r="E18">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
       </c>
       <c r="F18">
         <v>422.30599999999998</v>
@@ -813,19 +1034,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>18</v>
+        <v>20161115</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>96</v>
-      </c>
-      <c r="E19">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>96</v>
       </c>
       <c r="F19">
         <v>-370.14499999999998</v>
@@ -833,19 +1054,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>19</v>
+        <v>20161115</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>96</v>
-      </c>
-      <c r="E20">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
       </c>
       <c r="F20">
         <v>-496.58199999999999</v>
@@ -853,19 +1074,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>20</v>
+        <v>20161115</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>96</v>
-      </c>
-      <c r="E21">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
       </c>
       <c r="F21">
         <v>526.81299999999999</v>
@@ -873,19 +1094,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>21</v>
+        <v>20161115</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>96</v>
-      </c>
-      <c r="E22">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>79</v>
       </c>
       <c r="F22">
         <v>-286.38799999999998</v>
@@ -893,19 +1114,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>22</v>
+        <v>20161115</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>96</v>
-      </c>
-      <c r="E23">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
       </c>
       <c r="F23">
         <v>-49.167499999999997</v>
@@ -913,801 +1134,1001 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>23</v>
+        <v>20161115</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>96</v>
-      </c>
-      <c r="E24">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>99</v>
       </c>
       <c r="F24">
-        <v>3908.95</v>
+        <v>-290.68</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>24</v>
+        <v>20161115</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>96</v>
-      </c>
-      <c r="E25">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
       </c>
       <c r="F25">
-        <v>-264.67099999999999</v>
+        <v>192.262</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>25</v>
+        <v>20161115</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>96</v>
-      </c>
-      <c r="E26">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
       </c>
       <c r="F26">
-        <v>364.93299999999999</v>
+        <v>3908.95</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>26</v>
+        <v>20161115</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>96</v>
-      </c>
-      <c r="E27">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
       </c>
       <c r="F27">
-        <v>-84.950800000000001</v>
+        <v>-264.67099999999999</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>27</v>
+        <v>20161115</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
       </c>
       <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>96</v>
-      </c>
-      <c r="E28">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
       </c>
       <c r="F28">
-        <v>-347.16800000000001</v>
+        <v>364.93299999999999</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>28</v>
+        <v>20161115</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>96</v>
-      </c>
-      <c r="E29">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>94</v>
       </c>
       <c r="F29">
-        <v>74.122699999999995</v>
+        <v>-84.950800000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>29</v>
+        <v>20161115</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>96</v>
-      </c>
-      <c r="E30">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>95</v>
       </c>
       <c r="F30">
-        <v>-204.71299999999999</v>
+        <v>-347.16800000000001</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>30</v>
+        <v>20161115</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>96</v>
-      </c>
-      <c r="E31">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>96</v>
       </c>
       <c r="F31">
-        <v>48.929400000000001</v>
+        <v>74.122699999999995</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>31</v>
+        <v>20161115</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>96</v>
-      </c>
-      <c r="E32">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
       </c>
       <c r="F32">
-        <v>621.50099999999998</v>
+        <v>-204.71299999999999</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>32</v>
+        <v>20161115</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>96</v>
-      </c>
-      <c r="E33">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>98</v>
       </c>
       <c r="F33">
-        <v>805.51199999999994</v>
+        <v>48.929400000000001</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>33</v>
+        <v>20161115</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>96</v>
-      </c>
-      <c r="E34">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>80</v>
       </c>
       <c r="F34">
-        <v>-190.471</v>
+        <v>621.50099999999998</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>34</v>
+        <v>20161115</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>96</v>
-      </c>
-      <c r="E35">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>80</v>
       </c>
       <c r="F35">
-        <v>-307.87799999999999</v>
+        <v>805.51199999999994</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>35</v>
+        <v>20161115</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>96</v>
-      </c>
-      <c r="E36">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>99</v>
       </c>
       <c r="F36">
-        <v>-291.05399999999997</v>
+        <v>-155.928</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>36</v>
+        <v>20161115</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>96</v>
-      </c>
-      <c r="E37">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>99</v>
       </c>
       <c r="F37">
-        <v>23.320499999999999</v>
+        <v>-238.76499999999999</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>37</v>
+        <v>20161115</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>96</v>
-      </c>
-      <c r="E38">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>83</v>
       </c>
       <c r="F38">
-        <v>-282.17200000000003</v>
+        <v>-190.471</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>38</v>
+        <v>20161115</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>96</v>
-      </c>
-      <c r="E39">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>84</v>
       </c>
       <c r="F39">
-        <v>-303.39</v>
+        <v>-307.87799999999999</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>39</v>
+        <v>20161115</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>96</v>
-      </c>
-      <c r="E40">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>85</v>
       </c>
       <c r="F40">
-        <v>-475.74099999999999</v>
+        <v>-291.05399999999997</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>40</v>
+        <v>20161115</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>96</v>
-      </c>
-      <c r="E41">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>86</v>
       </c>
       <c r="F41">
-        <v>482.678</v>
+        <v>23.320499999999999</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>41</v>
+        <v>20161115</v>
       </c>
       <c r="B42" t="s">
         <v>31</v>
       </c>
       <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>96</v>
-      </c>
-      <c r="E42">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>87</v>
       </c>
       <c r="F42">
-        <v>1096020</v>
+        <v>-282.17200000000003</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>42</v>
+        <v>20161115</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>96</v>
-      </c>
-      <c r="E43">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>88</v>
       </c>
       <c r="F43">
-        <v>1028630</v>
+        <v>-303.39</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
+        <v>20161115</v>
+      </c>
+      <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
-        <v>6</v>
-      </c>
       <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44">
-        <v>96</v>
-      </c>
-      <c r="E44">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>89</v>
       </c>
       <c r="F44">
-        <v>60.828099999999999</v>
+        <v>-475.74099999999999</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>44</v>
+        <v>20161115</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>96</v>
-      </c>
-      <c r="E45">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>90</v>
       </c>
       <c r="F45">
-        <v>332.34399999999999</v>
+        <v>482.678</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>45</v>
+        <v>20161115</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46">
-        <v>96</v>
-      </c>
-      <c r="E46">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
+        <v>100</v>
       </c>
       <c r="F46">
-        <v>3863.74</v>
+        <v>1096020</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>46</v>
+        <v>20161115</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47">
-        <v>96</v>
-      </c>
-      <c r="E47">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>100</v>
       </c>
       <c r="F47">
-        <v>2818.24</v>
+        <v>1028630</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>47</v>
+        <v>20161115</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
-        <v>96</v>
-      </c>
-      <c r="E48">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>99</v>
       </c>
       <c r="F48">
-        <v>582.08000000000004</v>
+        <v>-39.253100000000003</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>48</v>
+        <v>20161115</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
-        <v>96</v>
-      </c>
-      <c r="E49">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>99</v>
       </c>
       <c r="F49">
-        <v>583.11699999999996</v>
+        <v>-140.6</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>49</v>
+        <v>20161115</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50">
-        <v>96</v>
-      </c>
-      <c r="E50">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>83</v>
       </c>
       <c r="F50">
-        <v>-137.39699999999999</v>
+        <v>60.828099999999999</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>50</v>
+        <v>20161115</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51">
-        <v>96</v>
-      </c>
-      <c r="E51">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>84</v>
       </c>
       <c r="F51">
-        <v>545.60199999999998</v>
+        <v>332.34399999999999</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>51</v>
+        <v>20161115</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>96</v>
-      </c>
-      <c r="E52">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>85</v>
       </c>
       <c r="F52">
-        <v>216380</v>
+        <v>3863.74</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>52</v>
+        <v>20161115</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53">
-        <v>96</v>
-      </c>
-      <c r="E53">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>86</v>
       </c>
       <c r="F53">
-        <v>91222.6</v>
+        <v>2818.24</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>22</v>
+        <v>20161115</v>
+      </c>
+      <c r="B54" t="s">
+        <v>32</v>
       </c>
       <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>96</v>
-      </c>
-      <c r="E54">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>87</v>
       </c>
       <c r="F54">
-        <v>4392890</v>
+        <v>582.08000000000004</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>22</v>
+        <v>20161115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>35</v>
       </c>
       <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55">
-        <v>96</v>
-      </c>
-      <c r="E55">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>88</v>
       </c>
       <c r="F55">
-        <v>4195230</v>
+        <v>583.11699999999996</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>23</v>
+        <v>20161115</v>
+      </c>
+      <c r="B56" t="s">
+        <v>44</v>
       </c>
       <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>96</v>
-      </c>
-      <c r="E56">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>89</v>
       </c>
       <c r="F56">
-        <v>549184</v>
+        <v>-137.39699999999999</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>23</v>
+        <v>20161115</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
       </c>
       <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57">
-        <v>96</v>
-      </c>
-      <c r="E57">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>90</v>
       </c>
       <c r="F57">
-        <v>972067</v>
+        <v>545.60199999999998</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>24</v>
+        <v>20161115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
       </c>
       <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>96</v>
-      </c>
-      <c r="E58">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>82</v>
       </c>
       <c r="F58">
-        <v>627501</v>
+        <v>216380</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>24</v>
+        <v>20161115</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
       </c>
       <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59">
-        <v>96</v>
-      </c>
-      <c r="E59">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>82</v>
       </c>
       <c r="F59">
-        <v>930836</v>
+        <v>91222.6</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>25</v>
+        <v>20161115</v>
+      </c>
+      <c r="B60" t="s">
+        <v>68</v>
       </c>
       <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>96</v>
-      </c>
-      <c r="E60">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>99</v>
       </c>
       <c r="F60">
-        <v>728666</v>
+        <v>110.471</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>25</v>
+        <v>20161115</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
       </c>
       <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61">
-        <v>96</v>
-      </c>
-      <c r="E61">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>99</v>
       </c>
       <c r="F61">
-        <v>485235</v>
+        <v>-53.646500000000003</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>26</v>
+        <v>20161115</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
       </c>
       <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62">
-        <v>96</v>
-      </c>
-      <c r="E62">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F62">
-        <v>310613</v>
+        <v>392.78500000000003</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>26</v>
+        <v>20161115</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
       </c>
       <c r="C63">
-        <v>2</v>
-      </c>
-      <c r="D63">
-        <v>96</v>
-      </c>
-      <c r="E63">
-        <v>20161115</v>
+        <v>96</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F63">
+        <v>2031.78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>20161115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64">
+        <v>96</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F64">
+        <v>4392890</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>20161115</v>
+      </c>
+      <c r="B65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65">
+        <v>96</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F65">
+        <v>4195230</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>20161115</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66">
+        <v>96</v>
+      </c>
+      <c r="D66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F66">
+        <v>549184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>20161115</v>
+      </c>
+      <c r="B67" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67">
+        <v>96</v>
+      </c>
+      <c r="D67" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F67">
+        <v>972067</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>20161115</v>
+      </c>
+      <c r="B68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68">
+        <v>96</v>
+      </c>
+      <c r="D68" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F68">
+        <v>627501</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>20161115</v>
+      </c>
+      <c r="B69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69">
+        <v>96</v>
+      </c>
+      <c r="D69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F69">
+        <v>930836</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>20161115</v>
+      </c>
+      <c r="B70" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70">
+        <v>96</v>
+      </c>
+      <c r="D70" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F70">
+        <v>728666</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>20161115</v>
+      </c>
+      <c r="B71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71">
+        <v>96</v>
+      </c>
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F71">
+        <v>485235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>20161115</v>
+      </c>
+      <c r="B72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72">
+        <v>96</v>
+      </c>
+      <c r="D72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72">
+        <v>310613</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>20161115</v>
+      </c>
+      <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73">
+        <v>96</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F73">
         <v>90436.800000000003</v>
       </c>
     </row>

</xml_diff>